<commit_message>
update: 1/12/2025: Update last 30 days report
</commit_message>
<xml_diff>
--- a/Consultant_Active_Reports/Active_Candidates_Ada_Sitnik.xlsx
+++ b/Consultant_Active_Reports/Active_Candidates_Ada_Sitnik.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -555,49 +555,49 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>768</v>
+        <v>773</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Adaptive6</t>
+          <t>CodeRabbit</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Senior Sales Engineer (US)</t>
+          <t>Sales Engineer Bay Area/Boston</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Anthony Joanes</t>
+          <t>Aryan Abdolhosseini</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>CV Sent</t>
+          <t>1st Interview</t>
         </is>
       </c>
       <c r="F5" s="2" t="n">
-        <v>45966</v>
+        <v>45973</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>773</v>
+        <v>784</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>CodeRabbit</t>
+          <t>Chainguard</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Sales Engineer Bay Area/Boston</t>
+          <t>RVP SF/PNW</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Aryan Abdolhosseini</t>
+          <t>Alex Biller</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -606,82 +606,82 @@
         </is>
       </c>
       <c r="F6" s="2" t="n">
-        <v>45973</v>
+        <v>45967</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>784</v>
+        <v>793</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Chainguard</t>
+          <t>Cognition AI</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>RVP SF/PNW</t>
+          <t>Forward Deployed Engineer / Sales Engineer (US)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Alex Biller</t>
+          <t>Ben Ogden</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1st Interview</t>
+          <t>CV Sent</t>
         </is>
       </c>
       <c r="F7" s="2" t="n">
-        <v>45967</v>
+        <v>45965</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>787</v>
+        <v>800</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Allium</t>
+          <t>Legion Security</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Solutions Engineer</t>
+          <t>TAM/TSM</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Ryan King</t>
+          <t>Matthew Fay</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>3rd Interview</t>
+          <t>CV Sent</t>
         </is>
       </c>
       <c r="F8" s="2" t="n">
-        <v>45988</v>
+        <v>45968</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>793</v>
+        <v>800</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Cognition AI</t>
+          <t>Legion Security</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Forward Deployed Engineer / Sales Engineer (US)</t>
+          <t>TAM/TSM</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Ben Ogden</t>
+          <t>Robert Blood</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -690,62 +690,6 @@
         </is>
       </c>
       <c r="F9" s="2" t="n">
-        <v>45965</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>800</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Legion Security</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>TAM/TSM</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Matthew Fay</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>CV Sent</t>
-        </is>
-      </c>
-      <c r="F10" s="2" t="n">
-        <v>45968</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>800</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Legion Security</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>TAM/TSM</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Robert Blood</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>CV Sent</t>
-        </is>
-      </c>
-      <c r="F11" s="2" t="n">
         <v>45968</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: 1/12/2025: Fix the algorithm/conditions on filtering the status of candidates
</commit_message>
<xml_diff>
--- a/Consultant_Active_Reports/Active_Candidates_Ada_Sitnik.xlsx
+++ b/Consultant_Active_Reports/Active_Candidates_Ada_Sitnik.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -555,26 +555,26 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>773</v>
+        <v>708</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>CodeRabbit</t>
+          <t>Dash0</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Sales Engineer Bay Area/Boston</t>
+          <t>Sales Engineer (US) x 3</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Aryan Abdolhosseini</t>
+          <t>Sean Guillen</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1st Interview</t>
+          <t>2nd Interview</t>
         </is>
       </c>
       <c r="F5" s="2" t="n">
@@ -583,16 +583,16 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>784</v>
+        <v>727</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Chainguard</t>
+          <t>Rox</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>RVP SF/PNW</t>
+          <t>RVP Sales West (SF)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -602,94 +602,178 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1st Interview</t>
+          <t>2nd Interview</t>
         </is>
       </c>
       <c r="F6" s="2" t="n">
-        <v>45967</v>
+        <v>45989</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>793</v>
+        <v>730</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Cognition AI</t>
+          <t>PointFive</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Forward Deployed Engineer / Sales Engineer (US)</t>
+          <t>PointFive SE EST</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Ben Ogden</t>
+          <t>Tony Bermeo</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>CV Sent</t>
+          <t>1st Interview</t>
         </is>
       </c>
       <c r="F7" s="2" t="n">
-        <v>45965</v>
+        <v>45967</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>800</v>
+        <v>773</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Legion Security</t>
+          <t>CodeRabbit</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>TAM/TSM</t>
+          <t>Sales Engineer Bay Area/Boston</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Matthew Fay</t>
+          <t>Aryan Abdolhosseini</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>CV Sent</t>
+          <t>1st Interview</t>
         </is>
       </c>
       <c r="F8" s="2" t="n">
-        <v>45968</v>
+        <v>45973</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
+        <v>784</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Chainguard</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>RVP SF/PNW</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Alex Biller</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>1st Interview</t>
+        </is>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>45967</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>793</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Cognition AI</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Forward Deployed Engineer / Sales Engineer (US)</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Ben Ogden</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>CV Sent</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>45965</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
         <v>800</v>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B11" t="inlineStr">
         <is>
           <t>Legion Security</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>TAM/TSM</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Matthew Fay</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>CV Sent</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="n">
+        <v>45968</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>800</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Legion Security</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>TAM/TSM</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
         <is>
           <t>Robert Blood</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>CV Sent</t>
         </is>
       </c>
-      <c r="F9" s="2" t="n">
+      <c r="F12" s="2" t="n">
         <v>45968</v>
       </c>
     </row>

</xml_diff>

<commit_message>
19/12/2025: Update the list
</commit_message>
<xml_diff>
--- a/Consultant_Active_Reports/Active_Candidates_Ada_Sitnik.xlsx
+++ b/Consultant_Active_Reports/Active_Candidates_Ada_Sitnik.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -501,12 +501,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Connor Lutz</t>
+          <t>Eddie Powers</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>1st Interview</t>
+          <t>2nd Interview</t>
         </is>
       </c>
     </row>
@@ -526,87 +526,87 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Eddie Powers</t>
+          <t>Jathan Prince</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2nd Interview</t>
+          <t>3rd Interview</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>580</v>
+        <v>708</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Legion Security</t>
+          <t>Dash0</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Sales Engineer (US)</t>
+          <t>Sales Engineer (US) x 3</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Jathan Prince</t>
+          <t>Sean Guillen</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>3rd Interview</t>
+          <t>4th Interview</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>708</v>
+        <v>730</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Dash0</t>
+          <t>PointFive</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Sales Engineer (US) x 3</t>
+          <t>PointFive SE EST</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Sean Guillen</t>
+          <t>Yuval Shkedi</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>4th Interview</t>
+          <t>3rd Interview</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>730</v>
+        <v>773</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>PointFive</t>
+          <t>CodeRabbit</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>PointFive SE EST</t>
+          <t>Sales Engineer Bay Area/Boston</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Yuval Shkedi</t>
+          <t>Peter Yoakum</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>3rd Interview</t>
+          <t>CV Sent</t>
         </is>
       </c>
     </row>
@@ -626,12 +626,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Peter Yoakum</t>
+          <t>Seth King</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>CV Sent</t>
+          <t>3rd Interview</t>
         </is>
       </c>
     </row>
@@ -651,12 +651,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Seth King</t>
+          <t>Seth Meldon</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2nd Interview</t>
+          <t>CV Sent</t>
         </is>
       </c>
     </row>
@@ -707,6 +707,31 @@
       <c r="E11" t="inlineStr">
         <is>
           <t>1st Interview</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>836</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Spectro Cloud</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>CSE EMEA</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Syed Imran</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>CV Sent</t>
         </is>
       </c>
     </row>

</xml_diff>